<commit_message>
added results from lag experiments
</commit_message>
<xml_diff>
--- a/output/Results.xlsx
+++ b/output/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb6e38027d4efde7/Northwestern/MSDS 458/Final Project/Fantasy-Forecasting/output/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb6e38027d4efde7/Northwestern/MSDS 458/Final Project/Fantasy-Forecasting/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="13_ncr:1_{AD356E9D-7F51-4BAA-B0BB-DD0CFAC12127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0A2314B-E4D6-4B21-A9D9-23E609B405AE}"/>
+  <xr:revisionPtr revIDLastSave="377" documentId="13_ncr:1_{AD356E9D-7F51-4BAA-B0BB-DD0CFAC12127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9CA075E-25C3-4737-9984-40065A1B0CCA}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{DDE0EE78-AAB8-4B08-85D7-99BC62FE6A27}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="68">
   <si>
     <t>Experiment #</t>
   </si>
@@ -226,6 +226,21 @@
   </si>
   <si>
     <t>48 seconds</t>
+  </si>
+  <si>
+    <t>included 1, 2, and 3 season lags</t>
+  </si>
+  <si>
+    <t>53 seconds</t>
+  </si>
+  <si>
+    <t>37 seconds</t>
+  </si>
+  <si>
+    <t>65 seconds</t>
+  </si>
+  <si>
+    <t>1221 seconds</t>
   </si>
 </sst>
 </file>
@@ -599,8 +614,8 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1782,6 +1797,202 @@
         <v>46716</v>
       </c>
     </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I34" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34">
+        <v>16394</v>
+      </c>
+      <c r="K34">
+        <v>12750</v>
+      </c>
+      <c r="L34">
+        <v>13877</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I35" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35">
+        <v>16325</v>
+      </c>
+      <c r="K35">
+        <v>13270</v>
+      </c>
+      <c r="L35">
+        <v>14176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36">
+        <v>16562</v>
+      </c>
+      <c r="K36">
+        <v>12760</v>
+      </c>
+      <c r="L36">
+        <v>13732</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G37">
+        <v>8</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37">
+        <v>16263</v>
+      </c>
+      <c r="K37">
+        <v>12706</v>
+      </c>
+      <c r="L37">
+        <v>13715</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G38">
+        <v>111</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I38" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38">
+        <v>48682</v>
+      </c>
+      <c r="K38">
+        <v>37599</v>
+      </c>
+      <c r="L38">
+        <v>48510</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H43">
+        <f>SQRT(12750)</f>
+        <v>112.91589790636215</v>
+      </c>
+    </row>
     <row r="1048576" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F1048576" s="2"/>
     </row>
@@ -1789,6 +2000,26 @@
   <autoFilter ref="A1:L18" xr:uid="{00AA1C50-1ECE-4022-AE12-381232E75728}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L1:L2 L21">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L10 L12:L16 L19">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1799,16 +2030,8 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L10 L12:L16 L19">
+  <conditionalFormatting sqref="L3:L10 L12:L16 L19 L21">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1820,7 +2043,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L10 L12:L16 L19 L21">
+  <conditionalFormatting sqref="L3:L16">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1832,7 +2055,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L16">
+  <conditionalFormatting sqref="L17:L18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1868,7 +2091,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L17:L18">
+  <conditionalFormatting sqref="L3:L18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1880,20 +2103,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L18">
+  <conditionalFormatting sqref="L2:L19 L21:L26">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L19 L21:L26">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1902,7 +2113,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L33">
+  <conditionalFormatting sqref="L2:L38">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K33 K35:K36 K38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1914,7 +2137,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K33">
+  <conditionalFormatting sqref="K2:K38">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
1871-1960 data and lags 4 + 5
</commit_message>
<xml_diff>
--- a/output/Results.xlsx
+++ b/output/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb6e38027d4efde7/Northwestern/MSDS 458/Final Project/Fantasy-Forecasting/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="13_ncr:1_{AD356E9D-7F51-4BAA-B0BB-DD0CFAC12127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9CA075E-25C3-4737-9984-40065A1B0CCA}"/>
+  <xr:revisionPtr revIDLastSave="447" documentId="13_ncr:1_{AD356E9D-7F51-4BAA-B0BB-DD0CFAC12127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{862DCB32-0C0F-4FB7-A935-1BEC1D861EFB}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{DDE0EE78-AAB8-4B08-85D7-99BC62FE6A27}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="74">
   <si>
     <t>Experiment #</t>
   </si>
@@ -241,6 +241,24 @@
   </si>
   <si>
     <t>1221 seconds</t>
+  </si>
+  <si>
+    <t>106 seconds</t>
+  </si>
+  <si>
+    <t>included 1, 2, and 3 season lags, 1871-1960 for training</t>
+  </si>
+  <si>
+    <t>included 1-5 season lags</t>
+  </si>
+  <si>
+    <t>58 seconds</t>
+  </si>
+  <si>
+    <t>43 seconds</t>
+  </si>
+  <si>
+    <t>33 seconds</t>
   </si>
 </sst>
 </file>
@@ -614,8 +632,8 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1987,10 +2005,232 @@
         <v>48510</v>
       </c>
     </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I39" t="s">
+        <v>69</v>
+      </c>
+      <c r="J39">
+        <v>10325</v>
+      </c>
+      <c r="K39">
+        <v>12954</v>
+      </c>
+      <c r="L39">
+        <v>13763</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I40" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40">
+        <v>16380</v>
+      </c>
+      <c r="K40">
+        <v>12737</v>
+      </c>
+      <c r="L40">
+        <v>13901</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" t="s">
+        <v>70</v>
+      </c>
+      <c r="J41">
+        <v>17559</v>
+      </c>
+      <c r="K41">
+        <v>12835</v>
+      </c>
+      <c r="L41">
+        <v>13855</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I42" t="s">
+        <v>70</v>
+      </c>
+      <c r="J42">
+        <v>18279</v>
+      </c>
+      <c r="K42">
+        <v>12890</v>
+      </c>
+      <c r="L42">
+        <v>13796</v>
+      </c>
+    </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="H43">
-        <f>SQRT(12750)</f>
-        <v>112.91589790636215</v>
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" t="s">
+        <v>70</v>
+      </c>
+      <c r="J43">
+        <v>16469</v>
+      </c>
+      <c r="K43">
+        <v>12784</v>
+      </c>
+      <c r="L43">
+        <v>13854</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44" t="s">
+        <v>70</v>
+      </c>
+      <c r="J44">
+        <v>16559</v>
+      </c>
+      <c r="K44">
+        <v>12884</v>
+      </c>
+      <c r="L44">
+        <v>13776</v>
       </c>
     </row>
     <row r="1048576" spans="6:6" x14ac:dyDescent="0.45">
@@ -2000,6 +2240,26 @@
   <autoFilter ref="A1:L18" xr:uid="{00AA1C50-1ECE-4022-AE12-381232E75728}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L1:L2 L21">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L10 L12:L16 L19">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2010,16 +2270,8 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L10 L12:L16 L19">
+  <conditionalFormatting sqref="L3:L10 L12:L16 L19 L21">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2031,7 +2283,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L10 L12:L16 L19 L21">
+  <conditionalFormatting sqref="L3:L16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2043,7 +2295,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L16">
+  <conditionalFormatting sqref="L17:L18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2079,7 +2331,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L17:L18">
+  <conditionalFormatting sqref="L3:L18">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2091,20 +2343,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L18">
+  <conditionalFormatting sqref="L2:L19 L21:L26">
     <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L19 L21:L26">
-    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2114,6 +2354,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L38">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K33 K35:K36 K38">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2125,7 +2377,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K33 K35:K36 K38">
+  <conditionalFormatting sqref="K2:K38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2137,7 +2389,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K38">
+  <conditionalFormatting sqref="K2:L44">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>